<commit_message>
Editamos casos de prueba.xlsx
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Samuel\Programacion samuel\Python\Preentrega_3\Preentrega3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C84EAE93-B1C0-4238-97E7-46DCB4F470E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D415F88A-4A1A-4DA6-8AF9-0D3D7ABB8324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Probado en: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmar que la funcionalidades probadas operan correctamente en el entorno de prueba, de acuerdo con los requisitos especificados. </t>
   </si>
   <si>
     <r>
@@ -198,11 +201,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> http://localhost:8000/users/autor/nuevo</t>
+      <t xml:space="preserve"> http://localhost:8000/autor/nuevo</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirmar que la funcionalidades probadas operan correctamente en el entorno de prueba, de acuerdo con los requisitos especificados. </t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>